<commit_message>
Gift Logs Merged - 23 April 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_T1513_ClientGiftPre_ApprovalPage_AddingaRecipientToTheSelectedRecipientSection.xlsx
+++ b/TestData/LV_T1513_ClientGiftPre_ApprovalPage_AddingaRecipientToTheSelectedRecipientSection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9A146E-EF22-4AFB-B9DA-6930764CEA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075083CB-9FEC-4DC8-8779-D65AEE84D74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="708" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -542,17 +542,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -571,17 +571,17 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -599,14 +599,14 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -624,21 +624,21 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -673,7 +673,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -722,13 +722,13 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -736,7 +736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -744,7 +744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -752,7 +752,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -760,13 +760,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -774,13 +774,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -788,13 +788,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -816,13 +816,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -830,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -838,7 +838,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -846,12 +846,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -869,16 +869,16 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.88671875" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -886,7 +886,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -894,7 +894,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -902,7 +902,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -910,7 +910,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -918,62 +918,62 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -991,32 +991,32 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Merge - GiftLogs - Tcs. Pages & Test Data - 9th Oct 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_T1513_ClientGiftPre_ApprovalPage_AddingaRecipientToTheSelectedRecipientSection.xlsx
+++ b/TestData/LV_T1513_ClientGiftPre_ApprovalPage_AddingaRecipientToTheSelectedRecipientSection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075083CB-9FEC-4DC8-8779-D65AEE84D74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0CD8B4-CBF2-47E1-A8FD-1A4457A7EA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="708" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -142,9 +142,6 @@
     <t>Congratulations</t>
   </si>
   <si>
-    <t>StdUser</t>
-  </si>
-  <si>
     <t>SubmittedFor</t>
   </si>
   <si>
@@ -205,7 +202,10 @@
     <t>Giftlog</t>
   </si>
   <si>
-    <t>Melissa Zatta</t>
+    <t>Julie Carthane</t>
+  </si>
+  <si>
+    <t>CF FinancialUser</t>
   </si>
 </sst>
 </file>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,12 +549,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>57</v>
+      <c r="A2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -578,12 +578,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -603,12 +603,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -621,7 +621,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +643,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>25</v>
@@ -652,7 +652,7 @@
         <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>28</v>
@@ -677,17 +677,17 @@
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>57</v>
+      <c r="B2" t="s">
+        <v>56</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
         <v>29</v>
@@ -696,10 +696,10 @@
         <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J2" t="s">
         <v>21</v>
@@ -868,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -880,102 +880,102 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -998,27 +998,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>